<commit_message>
replace ~ with 0
</commit_message>
<xml_diff>
--- a/Jarak antar tempat wisata di Bandung.xlsx
+++ b/Jarak antar tempat wisata di Bandung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB3AD6A2-FF0F-4960-A888-21E5DA10E9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED75557-5992-44E6-8BBE-5042601831E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A462356A-2120-4273-9707-A9683E8D1F3D}"/>
   </bookViews>
@@ -34,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="65">
   <si>
     <t>i/j</t>
-  </si>
-  <si>
-    <t>~</t>
   </si>
   <si>
     <t>7.1</t>
@@ -597,7 +594,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,35 +638,35 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
+      <c r="B2" s="1">
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="J2" s="1">
         <v>34</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -677,34 +674,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H3" s="1">
         <v>14</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -712,34 +709,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -747,19 +744,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="G5" s="1">
         <v>13</v>
@@ -768,13 +765,13 @@
         <v>17</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -782,34 +779,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1">
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -817,34 +814,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="J7" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -852,34 +849,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1">
         <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>1</v>
+        <v>52</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -887,34 +884,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -922,34 +919,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" s="1">
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -957,34 +954,34 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1">
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="1">
         <v>14.1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>1</v>
+      <c r="K11" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>